<commit_message>
Version 3.0 (BETA) Build 3017
- Add code for generate result data file compatible with AMASS Version 2.0
- Fix bug/Change request regarding team internal review on Annex C layout/wording etc. as well as comment from MOPH meeting.
</commit_message>
<xml_diff>
--- a/AMASS3.0/Configuration/Configuration.xlsx
+++ b/AMASS3.0/Configuration/Configuration.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chalida\Documents\AMASSv2.0.15_testRun_20221006\AMASSv2.0\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ONGWORK\TEST\AMASS3.0B3014\AMASS3.0-Lite-main\AMASS3.0\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ECD106-5D54-436D-B371-B291473323AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" xr2:uid="{3DDA365C-AA97-4E2E-9697-A1BDF02700BD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17736"/>
   </bookViews>
   <sheets>
     <sheet name="setting_parameters" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
   <si>
     <t>yes</t>
   </si>
@@ -253,12 +252,15 @@
   </si>
   <si>
     <t>Generating Supplementary report</t>
+  </si>
+  <si>
+    <t>amr_surveillance_annexC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -662,22 +664,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45545F2-22CD-4A3A-BC00-A16A1CE30C4E}">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -691,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -705,7 +707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -719,7 +721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -733,7 +735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -747,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -761,7 +763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -775,7 +777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -789,7 +791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -803,7 +805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -817,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
@@ -831,7 +833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
@@ -845,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -859,37 +861,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4 B15 B6:B13" xr:uid="{5D3F36E8-CADA-41F3-9440-01E296B334E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4 B16 B6:B14">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Version 3.0 (BETA) Build 3019
- Update regarding AMASS meeting on 14 Nov 2023
</commit_message>
<xml_diff>
--- a/AMASS3.0/Configuration/Configuration.xlsx
+++ b/AMASS3.0/Configuration/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ONGWORK\TEST\AMASS3.0B3014\AMASS3.0-Lite-main\AMASS3.0\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ONGWORK\TEST\AMASS3.0B3018\AMASS3.0-Lite-main\AMASS3.0\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>yes</t>
   </si>
@@ -255,6 +255,18 @@
   </si>
   <si>
     <t>amr_surveillance_annexC</t>
+  </si>
+  <si>
+    <t>flexible_days_before_admission_for_CO</t>
+  </si>
+  <si>
+    <t>0 (default): -1 (allow a specimen collected a calendar day before the hospital admission date as community-origin infection): -2 (allow a specimen collected two calendar days before the hospital admission date as community-origin infection)</t>
+  </si>
+  <si>
+    <t>flexibile_days_after_discharge_for_HO</t>
+  </si>
+  <si>
+    <t>0 (default): 1 (allow a specimen collected a calendar day after the hospital discharge date as hospital-origin infection): 2 (allow a specimen collected two calendar days after the hospital discharge date as hospital-origin infection)</t>
   </si>
 </sst>
 </file>
@@ -305,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -328,29 +340,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,226 +729,254 @@
       <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4 B16 B6:B14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B16 B18 B2:B4">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Version 3.0 Build 3030
[CR-022] Configuration - edit parameter options in dropdown list and typos
- Add and revise text in Method section
- Revise introduction in Section4-5
</commit_message>
<xml_diff>
--- a/AMASS3.0/Configuration/Configuration.xlsx
+++ b/AMASS3.0/Configuration/Configuration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AMASS3.0.28_minkdev\AMASS3.0-Lite-main\AMASS3.0\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AMASS3.0.30_minkdev\AMASS3.0-Lite-main\AMASS3.0\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44882E26-81B4-4087-B8C9-BA8BCFE5D6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90F26CA-459B-4B98-9473-AC5107576EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setting_parameters" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="46">
   <si>
     <t>yes</t>
   </si>
@@ -123,21 +123,6 @@
     <t>UniformTime</t>
   </si>
   <si>
-    <t>profiling_minimum_resistant_isolate_for_antibiotic</t>
-  </si>
-  <si>
-    <t>profiling_minimum_susceptible_isolate_for_antibiotic</t>
-  </si>
-  <si>
-    <t>profiling_maximum_resistant_isolate_for_antibiotic</t>
-  </si>
-  <si>
-    <t>profiling_maximum_tested_isolate_for_antibiotic</t>
-  </si>
-  <si>
-    <t>profiling_maximum_susceptible_isolate_for_antibiotic</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -313,18 +298,42 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Minimum proportion of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t xml:space="preserve">Maximum number of signal days of one cluster can be spanned. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF0E101A"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>tested isolate</t>
+      <t xml:space="preserve"> (default): maximum number of signal days for one cluster is 100 days; 90; 60; 45; 30; 15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Minimum number of isolates can be detected as one cluster. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
     </r>
     <r>
       <rPr>
@@ -334,7 +343,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> for selecting antibiotics in AMR profiling process. </t>
+      <t xml:space="preserve"> (default): Minimum number of isolates can be detected as one cluster is 2 isolates; 3; 4; 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Number of Monte-Carlo replications. </t>
     </r>
     <r>
       <rPr>
@@ -344,7 +358,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>90.1</t>
+      <t xml:space="preserve">9999 </t>
     </r>
     <r>
       <rPr>
@@ -354,23 +368,50 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (default) : antibiotic with tested isolates &gt;=90.01% of total isolates will be selected; 95.1; 85.1; 80.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Maximum proportion of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>(default); 999</t>
+    </r>
+  </si>
+  <si>
+    <t>Retrospective Space-Time</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Statistical model for cluster signals process. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UniformTime</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF0E101A"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>tested isolate</t>
+      <t xml:space="preserve"> (default); Space-Time Permutation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Analysis type for cluster signals process.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Retrospective Space-Time </t>
     </r>
     <r>
       <rPr>
@@ -380,7 +421,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> for selecting antibiotics in AMR profiling process. </t>
+      <t>(default); Prospective Space-Time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Maximum proportion of isolates in one cluster. </t>
     </r>
     <r>
       <rPr>
@@ -390,7 +436,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>100</t>
+      <t>50</t>
     </r>
     <r>
       <rPr>
@@ -400,344 +446,32 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (default) : antibiotic with tested isolates &lt;=100% of total isolates will be selected; 99; 95; 90</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Minimum proportion of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t xml:space="preserve"> (default): maximum proportion of isolates in a cluster is 50% of total isolates; 45; 40; 35; 30</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Minimum proportion of tested isolate for selecting antibiotics in AMR profiling process. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>90</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF0E101A"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">resistant isolate </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">for selecting antibiotics in AMR profiling process. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (default) : antibiotic with resistant isolates &gt;=0.01% of tested isolates will be selected; 0.5; 1.0; 5.0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Maximum proportion of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">resistant isolate </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">for selecting antibiotics in AMR profiling process. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>99.9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (default) : antibiotic with resistant isolates &lt;=99.9% of tested isolates will be selected; 99; 95; 90</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Minimum proportion of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>susceptible isolate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for selecting antibiotics in AMR profiling process. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (default) : antibiotic with susceptible isolates &gt;=0.01% of tested isolates will be selected; 0.5; 1.0; 5.0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Maximum proportion of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">susceptible isolate </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">for selecting antibiotics in AMR profiling process. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>99.9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (default) : antibiotic with susceptible isolates &lt;=99.9% of tested isolates will be selected; 99; 95; 90</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Maximum proportion of isolates in one cluster. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (default): maximum number of isolates in a cluster is 50% of total isolates; 45; 40; 35; 30</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Maximum number of signal days of one cluster can be spanned. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (default): maximum number of signal days for one cluster is 100 days; 90; 60; 45; 30; 15</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Minimum number of isolates can be detected as one cluster. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (default): Minimum number of isolates can be detected as one cluster is 2 isolates; 3; 4; 5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Number of Monte-Carlo replications. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">9999 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(default); 999</t>
-    </r>
-  </si>
-  <si>
-    <t>Retrospective Space-Time</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Statistical model for cluster signals process. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>UniformTime</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (default); Space-Time Permutation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Analysis type for cluster signals process.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Retrospective Space-Time </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0E101A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(default); Prospective Space-Time</t>
+      <t xml:space="preserve"> (default) : antibiotic with tested isolates &gt;=90% of total isolates will be selected; 100; 95; 85; 80</t>
     </r>
   </si>
 </sst>
@@ -745,7 +479,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,14 +505,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF0E101A"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -868,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -904,8 +630,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1221,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1261,7 +990,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -1275,7 +1004,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -1289,7 +1018,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -1303,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -1317,7 +1046,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1339,186 +1068,186 @@
         <v>24</v>
       </c>
       <c r="B8" s="10">
-        <v>90.1</v>
+        <v>90</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="10">
+        <v>50</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="10">
+        <v>100</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="10">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="12">
+        <v>9999</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="10">
-        <v>100</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="10">
-        <v>99.9</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="10">
-        <v>99.9</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="10">
-        <v>50</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="10">
-        <v>100</v>
+        <v>10</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D17" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="10">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>51</v>
+      <c r="D18" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="12">
-        <v>9999</v>
+      <c r="A19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>52</v>
+      <c r="D19" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>1</v>
+      <c r="A20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>0</v>
@@ -1527,12 +1256,12 @@
         <v>2</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>0</v>
@@ -1541,12 +1270,12 @@
         <v>2</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>0</v>
@@ -1555,12 +1284,12 @@
         <v>2</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>0</v>
@@ -1569,151 +1298,63 @@
         <v>2</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>40</v>
+      <c r="A25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <dataValidations count="14">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B31" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <phoneticPr fontId="5" type="noConversion"/>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B26 B2:B4 B16:B24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B8" xr:uid="{08CB2481-3ED1-42DC-A5A3-161FA9A92B81}">
-      <formula1>"90.1,95.1,85.1,80.1"</formula1>
+      <formula1>"100,95,90,85,80"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B9" xr:uid="{5121EA82-CDA5-46CF-B468-39C0EB032FB0}">
-      <formula1>"100.0,99.0,95.0,90.0"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B14" xr:uid="{CF777ABA-1CA8-4B41-9F3B-6990BDA95F42}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B9" xr:uid="{CF777ABA-1CA8-4B41-9F3B-6990BDA95F42}">
       <formula1>"Retrospective Space-Time, Prospective Space-Time"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B15" xr:uid="{AFC4672D-1860-4BE1-8973-D409B0CB1F5E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B10" xr:uid="{AFC4672D-1860-4BE1-8973-D409B0CB1F5E}">
       <formula1>"UniformTime, Space-Time Permutation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B16" xr:uid="{F77D9F99-0198-4EBC-8AAC-EACC52C51BEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B11" xr:uid="{F77D9F99-0198-4EBC-8AAC-EACC52C51BEB}">
       <formula1>"50, 45, 40, 35, 30"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B17" xr:uid="{A0B8A359-F98C-435E-AD41-DE46E5EE8A5D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B12" xr:uid="{A0B8A359-F98C-435E-AD41-DE46E5EE8A5D}">
       <formula1>"100, 90, 60, 45, 30, 15"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B18" xr:uid="{DE6ADC94-D58A-4C3D-8095-17A253B5AEA3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B13" xr:uid="{DE6ADC94-D58A-4C3D-8095-17A253B5AEA3}">
       <formula1>"2, 3, 4, 5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B19" xr:uid="{037C79DD-A3D6-4505-87C2-4E4E719084CE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B14" xr:uid="{037C79DD-A3D6-4505-87C2-4E4E719084CE}">
       <formula1>"9999, 999"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B12" xr:uid="{BE4A0C0D-646B-4CE2-B8A7-89C5A7C0F593}">
-      <formula1>"0.1,0.5,1.0,5.0"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B13" xr:uid="{448DD017-264B-4247-8A24-D750668A45B3}">
-      <formula1>"99.9,99.0,95.0,90.0"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B10" xr:uid="{08A25277-F09A-4771-BB61-EEFDB2148169}">
-      <formula1>"0.1,0.5,1.0,5.0"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B11" xr:uid="{D48F5F70-37AE-4BCB-A31D-1181FFBA1275}">
-      <formula1>"99.9,99.0,95.0,90.0"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B2 B3 B4 B21 B22 B23 B24 B25 B26 B27 B28 B29" xr:uid="{4BAA9748-A299-4246-A8B9-720043C09575}">
-      <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Version 3.0 Build 3031
Update default configuration of [flexible_days_before_admission_for_CO,flexibile_days_after_discharge_for_HO] from [0,0] to [-2,1] this will consider specimen with specimen date 2 days before admission period as CA origin and specimen with specimen date 1 day after admission period consider as HA
</commit_message>
<xml_diff>
--- a/AMASS3.0/Configuration/Configuration.xlsx
+++ b/AMASS3.0/Configuration/Configuration.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AMASS3.0.30_minkdev\AMASS3.0-Lite-main\AMASS3.0\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ONGWORK\GitHub\AMASS3.0-Lite\AMASS3.0\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90F26CA-459B-4B98-9473-AC5107576EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="setting_parameters" sheetId="1" r:id="rId1"/>
@@ -478,7 +477,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -949,23 +948,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.6328125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="48.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.6640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -979,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -993,7 +992,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1021,12 +1020,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="8">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>2</v>
@@ -1035,12 +1034,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1049,7 +1048,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1063,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1077,7 +1076,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1090,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -1119,7 +1118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -1133,7 +1132,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -1147,7 +1146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>30</v>
       </c>
@@ -1161,7 +1160,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1175,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
@@ -1189,7 +1188,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>10</v>
       </c>
@@ -1203,7 +1202,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1217,7 +1216,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>12</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>13</v>
       </c>
@@ -1245,7 +1244,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>14</v>
       </c>
@@ -1259,7 +1258,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>15</v>
       </c>
@@ -1273,7 +1272,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
@@ -1315,7 +1314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1332,28 +1331,28 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B26 B2:B4 B16:B24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B26 B2:B4 B16:B24">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B8" xr:uid="{08CB2481-3ED1-42DC-A5A3-161FA9A92B81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B8">
       <formula1>"100,95,90,85,80"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B9" xr:uid="{CF777ABA-1CA8-4B41-9F3B-6990BDA95F42}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B9">
       <formula1>"Retrospective Space-Time, Prospective Space-Time"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B10" xr:uid="{AFC4672D-1860-4BE1-8973-D409B0CB1F5E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B10">
       <formula1>"UniformTime, Space-Time Permutation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B11" xr:uid="{F77D9F99-0198-4EBC-8AAC-EACC52C51BEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B11">
       <formula1>"50, 45, 40, 35, 30"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B12" xr:uid="{A0B8A359-F98C-435E-AD41-DE46E5EE8A5D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B12">
       <formula1>"100, 90, 60, 45, 30, 15"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B13" xr:uid="{DE6ADC94-D58A-4C3D-8095-17A253B5AEA3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B13">
       <formula1>"2, 3, 4, 5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B14" xr:uid="{037C79DD-A3D6-4505-87C2-4E4E719084CE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B14">
       <formula1>"9999, 999"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Version 3.1 Build 3032
- Changing AMR profile generation from "using blood data for both blood and all specimens" to "using blood for blood profile" and "using all specimens for all specimen profiles"
- Adding "List of AST" to Supplementary report Annex C
- Adding options for "profiling_minimum_tested_isolate_for_antibiotic" in Configuration.xlsx
</commit_message>
<xml_diff>
--- a/AMASS3.0/Configuration/Configuration.xlsx
+++ b/AMASS3.0/Configuration/Configuration.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ONGWORK\GitHub\AMASS3.0-Lite\AMASS3.0\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chalida\Documents\GitHub\AMASS3.0-Lite\AMASS3.0\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6F0182-110D-41CF-BDAC-41BEBFCA7A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setting_parameters" sheetId="1" r:id="rId1"/>
@@ -477,7 +478,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -948,23 +949,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.6640625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="4"/>
+    <col min="1" max="1" width="48.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.6328125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -978,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -992,7 +993,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1006,7 +1007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1034,7 +1035,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1048,7 +1049,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1062,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
@@ -1104,7 +1105,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -1118,7 +1119,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>30</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>10</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1216,7 +1217,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>12</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>13</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>14</v>
       </c>
@@ -1258,7 +1259,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>15</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
@@ -1286,7 +1287,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1331,28 +1332,28 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B26 B2:B4 B16:B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B26 B2:B4 B16:B24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B8">
-      <formula1>"100,95,90,85,80"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B8" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>"100,95,90,85,80,75,70"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Retrospective Space-Time, Prospective Space-Time"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B10" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"UniformTime, Space-Time Permutation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B11" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"50, 45, 40, 35, 30"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B12" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"100, 90, 60, 45, 30, 15"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B13" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"2, 3, 4, 5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please click the &quot;Cancel&quot; button first, and then select a value from the dropdown list." sqref="B14" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"9999, 999"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>